<commit_message>
Edit line graph code Edit and added correlation for loop codes
</commit_message>
<xml_diff>
--- a/Datasets/SAMPLE - Arable land (% of land area).xlsx
+++ b/Datasets/SAMPLE - Arable land (% of land area).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashiq/Desktop/All Data Sets/Sample Data Set/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\PycharmProjects\gdp-analysis\Datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08CC504A-B4EB-1D42-ADE5-5931FE832CDD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32EAD720-0828-43E8-9B68-B1CD59A3A9F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="21600" xr2:uid="{81DAEDAA-4699-3647-82E1-ED4FF5A07DB6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{81DAEDAA-4699-3647-82E1-ED4FF5A07DB6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="34">
   <si>
     <t>Series Name</t>
   </si>
@@ -48,186 +48,6 @@
   </si>
   <si>
     <t>1960 [YR1960]</t>
-  </si>
-  <si>
-    <t>1961 [YR1961]</t>
-  </si>
-  <si>
-    <t>1962 [YR1962]</t>
-  </si>
-  <si>
-    <t>1963 [YR1963]</t>
-  </si>
-  <si>
-    <t>1964 [YR1964]</t>
-  </si>
-  <si>
-    <t>1965 [YR1965]</t>
-  </si>
-  <si>
-    <t>1966 [YR1966]</t>
-  </si>
-  <si>
-    <t>1967 [YR1967]</t>
-  </si>
-  <si>
-    <t>1968 [YR1968]</t>
-  </si>
-  <si>
-    <t>1969 [YR1969]</t>
-  </si>
-  <si>
-    <t>1970 [YR1970]</t>
-  </si>
-  <si>
-    <t>1971 [YR1971]</t>
-  </si>
-  <si>
-    <t>1972 [YR1972]</t>
-  </si>
-  <si>
-    <t>1973 [YR1973]</t>
-  </si>
-  <si>
-    <t>1974 [YR1974]</t>
-  </si>
-  <si>
-    <t>1975 [YR1975]</t>
-  </si>
-  <si>
-    <t>1976 [YR1976]</t>
-  </si>
-  <si>
-    <t>1977 [YR1977]</t>
-  </si>
-  <si>
-    <t>1978 [YR1978]</t>
-  </si>
-  <si>
-    <t>1979 [YR1979]</t>
-  </si>
-  <si>
-    <t>1980 [YR1980]</t>
-  </si>
-  <si>
-    <t>1981 [YR1981]</t>
-  </si>
-  <si>
-    <t>1982 [YR1982]</t>
-  </si>
-  <si>
-    <t>1983 [YR1983]</t>
-  </si>
-  <si>
-    <t>1984 [YR1984]</t>
-  </si>
-  <si>
-    <t>1985 [YR1985]</t>
-  </si>
-  <si>
-    <t>1986 [YR1986]</t>
-  </si>
-  <si>
-    <t>1987 [YR1987]</t>
-  </si>
-  <si>
-    <t>1988 [YR1988]</t>
-  </si>
-  <si>
-    <t>1989 [YR1989]</t>
-  </si>
-  <si>
-    <t>1990 [YR1990]</t>
-  </si>
-  <si>
-    <t>1991 [YR1991]</t>
-  </si>
-  <si>
-    <t>1992 [YR1992]</t>
-  </si>
-  <si>
-    <t>1993 [YR1993]</t>
-  </si>
-  <si>
-    <t>1994 [YR1994]</t>
-  </si>
-  <si>
-    <t>1995 [YR1995]</t>
-  </si>
-  <si>
-    <t>1996 [YR1996]</t>
-  </si>
-  <si>
-    <t>1997 [YR1997]</t>
-  </si>
-  <si>
-    <t>1998 [YR1998]</t>
-  </si>
-  <si>
-    <t>1999 [YR1999]</t>
-  </si>
-  <si>
-    <t>2000 [YR2000]</t>
-  </si>
-  <si>
-    <t>2001 [YR2001]</t>
-  </si>
-  <si>
-    <t>2002 [YR2002]</t>
-  </si>
-  <si>
-    <t>2003 [YR2003]</t>
-  </si>
-  <si>
-    <t>2004 [YR2004]</t>
-  </si>
-  <si>
-    <t>2005 [YR2005]</t>
-  </si>
-  <si>
-    <t>2006 [YR2006]</t>
-  </si>
-  <si>
-    <t>2007 [YR2007]</t>
-  </si>
-  <si>
-    <t>2008 [YR2008]</t>
-  </si>
-  <si>
-    <t>2009 [YR2009]</t>
-  </si>
-  <si>
-    <t>2010 [YR2010]</t>
-  </si>
-  <si>
-    <t>2011 [YR2011]</t>
-  </si>
-  <si>
-    <t>2012 [YR2012]</t>
-  </si>
-  <si>
-    <t>2013 [YR2013]</t>
-  </si>
-  <si>
-    <t>2014 [YR2014]</t>
-  </si>
-  <si>
-    <t>2015 [YR2015]</t>
-  </si>
-  <si>
-    <t>2016 [YR2016]</t>
-  </si>
-  <si>
-    <t>2017 [YR2017]</t>
-  </si>
-  <si>
-    <t>2018 [YR2018]</t>
-  </si>
-  <si>
-    <t>2019 [YR2019]</t>
-  </si>
-  <si>
-    <t>2020 [YR2020]</t>
   </si>
   <si>
     <t>Arable land (% of land area)</t>
@@ -350,8 +170,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -669,12 +492,12 @@
   <dimension ref="A1:BM14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="BJ33" sqref="BJ33"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -690,202 +513,202 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1">
+        <v>1960</v>
+      </c>
+      <c r="G1" s="1">
+        <v>1961</v>
+      </c>
+      <c r="H1" s="1">
+        <v>1962</v>
+      </c>
+      <c r="I1" s="1">
+        <v>1963</v>
+      </c>
+      <c r="J1" s="1">
+        <v>1964</v>
+      </c>
+      <c r="K1" s="1">
+        <v>1965</v>
+      </c>
+      <c r="L1" s="1">
+        <v>1966</v>
+      </c>
+      <c r="M1" s="1">
+        <v>1967</v>
+      </c>
+      <c r="N1" s="1">
+        <v>1968</v>
+      </c>
+      <c r="O1" s="1">
+        <v>1969</v>
+      </c>
+      <c r="P1" s="1">
+        <v>1970</v>
+      </c>
+      <c r="Q1" s="1">
+        <v>1971</v>
+      </c>
+      <c r="R1" s="1">
+        <v>1972</v>
+      </c>
+      <c r="S1" s="1">
+        <v>1973</v>
+      </c>
+      <c r="T1" s="1">
+        <v>1974</v>
+      </c>
+      <c r="U1" s="1">
+        <v>1975</v>
+      </c>
+      <c r="V1" s="1">
+        <v>1976</v>
+      </c>
+      <c r="W1" s="1">
+        <v>1977</v>
+      </c>
+      <c r="X1" s="1">
+        <v>1978</v>
+      </c>
+      <c r="Y1" s="1">
+        <v>1979</v>
+      </c>
+      <c r="Z1" s="1">
+        <v>1980</v>
+      </c>
+      <c r="AA1" s="1">
+        <v>1981</v>
+      </c>
+      <c r="AB1" s="1">
+        <v>1982</v>
+      </c>
+      <c r="AC1" s="1">
+        <v>1983</v>
+      </c>
+      <c r="AD1" s="1">
+        <v>1984</v>
+      </c>
+      <c r="AE1" s="1">
+        <v>1985</v>
+      </c>
+      <c r="AF1" s="1">
+        <v>1986</v>
+      </c>
+      <c r="AG1" s="1">
+        <v>1987</v>
+      </c>
+      <c r="AH1" s="1">
+        <v>1988</v>
+      </c>
+      <c r="AI1" s="1">
+        <v>1989</v>
+      </c>
+      <c r="AJ1" s="1">
+        <v>1990</v>
+      </c>
+      <c r="AK1" s="1">
+        <v>1991</v>
+      </c>
+      <c r="AL1" s="1">
+        <v>1992</v>
+      </c>
+      <c r="AM1" s="1">
+        <v>1993</v>
+      </c>
+      <c r="AN1" s="1">
+        <v>1994</v>
+      </c>
+      <c r="AO1" s="1">
+        <v>1995</v>
+      </c>
+      <c r="AP1" s="1">
+        <v>1996</v>
+      </c>
+      <c r="AQ1" s="1">
+        <v>1997</v>
+      </c>
+      <c r="AR1" s="1">
+        <v>1998</v>
+      </c>
+      <c r="AS1" s="1">
+        <v>1999</v>
+      </c>
+      <c r="AT1" s="1">
+        <v>2000</v>
+      </c>
+      <c r="AU1" s="1">
+        <v>2001</v>
+      </c>
+      <c r="AV1" s="1">
+        <v>2002</v>
+      </c>
+      <c r="AW1" s="1">
+        <v>2003</v>
+      </c>
+      <c r="AX1" s="1">
+        <v>2004</v>
+      </c>
+      <c r="AY1" s="1">
+        <v>2005</v>
+      </c>
+      <c r="AZ1" s="1">
+        <v>2006</v>
+      </c>
+      <c r="BA1" s="1">
+        <v>2007</v>
+      </c>
+      <c r="BB1" s="1">
+        <v>2008</v>
+      </c>
+      <c r="BC1" s="1">
+        <v>2009</v>
+      </c>
+      <c r="BD1" s="1">
+        <v>2010</v>
+      </c>
+      <c r="BE1" s="1">
+        <v>2011</v>
+      </c>
+      <c r="BF1" s="1">
+        <v>2012</v>
+      </c>
+      <c r="BG1" s="1">
+        <v>2013</v>
+      </c>
+      <c r="BH1" s="1">
+        <v>2014</v>
+      </c>
+      <c r="BI1" s="1">
+        <v>2015</v>
+      </c>
+      <c r="BJ1" s="1">
+        <v>2016</v>
+      </c>
+      <c r="BK1" s="1">
+        <v>2017</v>
+      </c>
+      <c r="BL1" s="1">
+        <v>2018</v>
+      </c>
+      <c r="BM1" s="1">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="2" spans="1:65" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AS1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AT1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AU1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AV1" t="s">
-        <v>47</v>
-      </c>
-      <c r="AW1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AY1" t="s">
-        <v>50</v>
-      </c>
-      <c r="AZ1" t="s">
-        <v>51</v>
-      </c>
-      <c r="BA1" t="s">
-        <v>52</v>
-      </c>
-      <c r="BB1" t="s">
-        <v>53</v>
-      </c>
-      <c r="BC1" t="s">
-        <v>54</v>
-      </c>
-      <c r="BD1" t="s">
-        <v>55</v>
-      </c>
-      <c r="BE1" t="s">
-        <v>56</v>
-      </c>
-      <c r="BF1" t="s">
-        <v>57</v>
-      </c>
-      <c r="BG1" t="s">
-        <v>58</v>
-      </c>
-      <c r="BH1" t="s">
-        <v>59</v>
-      </c>
-      <c r="BI1" t="s">
-        <v>60</v>
-      </c>
-      <c r="BJ1" t="s">
-        <v>61</v>
-      </c>
-      <c r="BK1" t="s">
-        <v>62</v>
-      </c>
-      <c r="BL1" t="s">
-        <v>63</v>
-      </c>
-      <c r="BM1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:65" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D2" t="s">
-        <v>68</v>
-      </c>
       <c r="E2" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="F2">
         <v>66.105861565644901</v>
@@ -1056,33 +879,33 @@
         <v>59.646692486268002</v>
       </c>
       <c r="BJ2" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="BK2" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="BL2" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="BM2" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>65</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="F3">
         <v>8.1589216034054601</v>
@@ -1253,33 +1076,33 @@
         <v>23.944661227385598</v>
       </c>
       <c r="BJ3" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="BK3" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="BL3" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="BM3" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>65</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>71</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>72</v>
+        <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="F4">
         <v>0.70403896035149005</v>
@@ -1450,33 +1273,33 @@
         <v>0.45806646216631602</v>
       </c>
       <c r="BJ4" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="BK4" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="BL4" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="BM4" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>65</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>73</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>74</v>
+        <v>14</v>
       </c>
       <c r="E5" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="F5">
         <v>2.6462825461167201</v>
@@ -1647,33 +1470,33 @@
         <v>9.6882799283094094</v>
       </c>
       <c r="BJ5" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="BK5" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="BL5" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="BM5" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>65</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>75</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>76</v>
+        <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="F6">
         <v>4.89555237301688</v>
@@ -1844,33 +1667,33 @@
         <v>1.7077946819498599</v>
       </c>
       <c r="BJ6" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="BK6" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="BL6" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="BM6" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>65</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>78</v>
+        <v>18</v>
       </c>
       <c r="E7" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="F7">
         <v>10.9285543099087</v>
@@ -2041,33 +1864,33 @@
         <v>12.664821089430299</v>
       </c>
       <c r="BJ7" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="BK7" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="BL7" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="BM7" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>65</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>79</v>
+        <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="E8" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="F8">
         <v>1.5226939970717399</v>
@@ -2238,33 +2061,33 @@
         <v>1.61054172767204</v>
       </c>
       <c r="BJ8" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="BK8" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="BL8" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="BM8" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>65</v>
+        <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>81</v>
+        <v>21</v>
       </c>
       <c r="D9" t="s">
-        <v>82</v>
+        <v>22</v>
       </c>
       <c r="E9" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="F9">
         <v>5.5816686251468903</v>
@@ -2435,33 +2258,33 @@
         <v>4.8472385428907199</v>
       </c>
       <c r="BJ9" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="BK9" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="BL9" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="BM9" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>65</v>
+        <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>83</v>
+        <v>23</v>
       </c>
       <c r="D10" t="s">
-        <v>84</v>
+        <v>24</v>
       </c>
       <c r="E10" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="F10">
         <v>5.2830188679245298</v>
@@ -2632,33 +2455,33 @@
         <v>9.1194968553459095</v>
       </c>
       <c r="BJ10" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="BK10" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="BL10" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="BM10" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>65</v>
+        <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>85</v>
+        <v>25</v>
       </c>
       <c r="D11" t="s">
-        <v>86</v>
+        <v>26</v>
       </c>
       <c r="E11" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="F11">
         <v>7.4712138525094502</v>
@@ -2829,33 +2652,33 @@
         <v>20.6557088863497</v>
       </c>
       <c r="BJ11" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="BK11" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="BL11" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="BM11" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>65</v>
+        <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>87</v>
+        <v>27</v>
       </c>
       <c r="D12" t="s">
-        <v>88</v>
+        <v>28</v>
       </c>
       <c r="E12" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="F12">
         <v>20.356632543208899</v>
@@ -3026,33 +2849,33 @@
         <v>32.903364716475203</v>
       </c>
       <c r="BJ12" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="BK12" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="BL12" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="BM12" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>65</v>
+        <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>89</v>
+        <v>29</v>
       </c>
       <c r="D13" t="s">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="E13" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="F13">
         <v>29.901381183165899</v>
@@ -3223,33 +3046,33 @@
         <v>26.481556072398401</v>
       </c>
       <c r="BJ13" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="BK13" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="BL13" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="BM13" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>65</v>
+        <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>91</v>
+        <v>31</v>
       </c>
       <c r="D14" t="s">
-        <v>92</v>
+        <v>32</v>
       </c>
       <c r="E14" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="F14">
         <v>4.4776119402985097</v>
@@ -3420,16 +3243,16 @@
         <v>0.789844838268139</v>
       </c>
       <c r="BJ14" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="BK14" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="BL14" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="BM14" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>